<commit_message>
solve magic number by using enum
</commit_message>
<xml_diff>
--- a/SchoolManagementApplication/resources/exportedschool.xlsx
+++ b/SchoolManagementApplication/resources/exportedschool.xlsx
@@ -38,7 +38,7 @@
     <t>Vinh Long</t>
   </si>
   <si>
-    <t>337829999,285656899</t>
+    <t>337829999</t>
   </si>
   <si>
     <t>nbk-qn</t>
@@ -108,7 +108,7 @@
     <col min="2" max="2" width="41.72265625" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="18.99609375" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="11.4296875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="21.65625" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="16.140625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -136,7 +136,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
refactor + test export data to text/excel file add sample export pdf/html file
</commit_message>
<xml_diff>
--- a/SchoolManagementApplication/resources/exportedschool.xlsx
+++ b/SchoolManagementApplication/resources/exportedschool.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>ID</t>
   </si>
@@ -27,27 +27,6 @@
   </si>
   <si>
     <t>Teacher's CMND</t>
-  </si>
-  <si>
-    <t>nbk-vl</t>
-  </si>
-  <si>
-    <t>Truong trung hoc Chuyen Nguyen Binh Khiem</t>
-  </si>
-  <si>
-    <t>Vinh Long</t>
-  </si>
-  <si>
-    <t>337829999</t>
-  </si>
-  <si>
-    <t>nbk-qn</t>
-  </si>
-  <si>
-    <t>Quang Ngai</t>
-  </si>
-  <si>
-    <t>334442222</t>
   </si>
 </sst>
 </file>
@@ -98,16 +77,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="41.72265625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="3.02734375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="6.48828125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="18.99609375" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="11.4296875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="8.39453125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="16.140625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
@@ -128,40 +107,6 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
fix wrong file name when export data to pdf
</commit_message>
<xml_diff>
--- a/SchoolManagementApplication/resources/exportedschool.xlsx
+++ b/SchoolManagementApplication/resources/exportedschool.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>ID</t>
   </si>
@@ -27,6 +27,27 @@
   </si>
   <si>
     <t>Teacher's CMND</t>
+  </si>
+  <si>
+    <t>nbk-vl</t>
+  </si>
+  <si>
+    <t>Truong trung hoc Chuyen Nguyen Binh Khiem</t>
+  </si>
+  <si>
+    <t>Vinh Long</t>
+  </si>
+  <si>
+    <t>337829999</t>
+  </si>
+  <si>
+    <t>nbk-qn</t>
+  </si>
+  <si>
+    <t>Quang Ngai</t>
+  </si>
+  <si>
+    <t>334442222</t>
   </si>
 </sst>
 </file>
@@ -77,16 +98,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="3.02734375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="6.48828125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="7.33203125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="41.72265625" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="18.99609375" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="8.39453125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="11.4296875" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="16.140625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
@@ -107,6 +128,40 @@
         <v>4</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>